<commit_message>
Fixed x-axis in charts.
</commit_message>
<xml_diff>
--- a/bitcoin_canvt.xlsx
+++ b/bitcoin_canvt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="990" windowWidth="23235" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="990" windowWidth="23235" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="chart" sheetId="2" r:id="rId1"/>
@@ -3818,7 +3818,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43101"/>
-          <c:min val="42005"/>
+          <c:min val="42006"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
@@ -3841,7 +3841,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="m/d/yyyy\ h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-409]mmm\ yyyy;@" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="2700000"/>
@@ -3913,7 +3913,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4234,7 +4234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B537"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>